<commit_message>
Cambios en los pesos de la calibracion
</commit_message>
<xml_diff>
--- a/data/templates/Canal_vargas/Comprobacion/PlantillaBaseQ2K.xlsx
+++ b/data/templates/Canal_vargas/Comprobacion/PlantillaBaseQ2K.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto_UB_2025\Modelo_Q2K_python\data\templates\Canal_vargas\Comprobacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BDF984-0AC7-407A-879E-2C143CE74272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C9BE78-16B4-4430-9BBE-41BFA24081EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7CAB968E-70C7-47AF-B60B-C3245F72BAF9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7CAB968E-70C7-47AF-B60B-C3245F72BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="REACHES" sheetId="1" r:id="rId1"/>
@@ -1148,8 +1148,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S10:S11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2229,9 +2229,7 @@
       <c r="G17" s="1">
         <v>19</v>
       </c>
-      <c r="H17" s="8">
-        <v>122184</v>
-      </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="1">
         <v>26.9</v>
       </c>
@@ -2505,8 +2503,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2617,7 +2615,7 @@
         <v>16.7</v>
       </c>
       <c r="G2" s="12">
-        <v>948</v>
+        <v>10000</v>
       </c>
       <c r="H2" s="11">
         <v>5</v>
@@ -2726,7 +2724,7 @@
         <v>16.5</v>
       </c>
       <c r="G4" s="12">
-        <v>28200</v>
+        <v>2820</v>
       </c>
       <c r="H4" s="13">
         <v>24</v>
@@ -2776,7 +2774,7 @@
         <v>14.3</v>
       </c>
       <c r="G5" s="12">
-        <v>20200</v>
+        <v>2020</v>
       </c>
       <c r="H5" s="13">
         <v>108</v>
@@ -2829,7 +2827,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="12">
-        <v>60500</v>
+        <v>6050</v>
       </c>
       <c r="H6" s="13">
         <v>102</v>
@@ -2879,7 +2877,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="12">
-        <v>10480</v>
+        <v>1048</v>
       </c>
       <c r="H7" s="13">
         <v>250</v>
@@ -2932,7 +2930,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="12">
-        <v>8640</v>
+        <v>864</v>
       </c>
       <c r="H8" s="13">
         <v>182</v>
@@ -2985,7 +2983,7 @@
         <v>22.5</v>
       </c>
       <c r="G9" s="12">
-        <v>34200</v>
+        <v>3420</v>
       </c>
       <c r="H9" s="13">
         <v>124</v>

</xml_diff>